<commit_message>
🍱 Add external identifiers
</commit_message>
<xml_diff>
--- a/project/excel/acr_harmonized_data_model.xlsx
+++ b/project/excel/acr_harmonized_data_model.xlsx
@@ -427,18 +427,23 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>external_id</t>
         </is>
       </c>
     </row>
@@ -453,7 +458,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -490,6 +495,11 @@
       <c r="F1" t="inlineStr">
         <is>
           <t>id</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>external_id</t>
         </is>
       </c>
     </row>
@@ -518,7 +528,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -560,6 +570,11 @@
       <c r="G1" t="inlineStr">
         <is>
           <t>id</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>external_id</t>
         </is>
       </c>
     </row>
@@ -579,7 +594,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -616,6 +631,11 @@
       <c r="F1" t="inlineStr">
         <is>
           <t>id</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>external_id</t>
         </is>
       </c>
     </row>
@@ -635,7 +655,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -664,6 +684,11 @@
           <t>id</t>
         </is>
       </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>external_id</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -676,7 +701,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -713,6 +738,11 @@
       <c r="F1" t="inlineStr">
         <is>
           <t>id</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>external_id</t>
         </is>
       </c>
     </row>
@@ -735,7 +765,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -769,6 +799,11 @@
           <t>id</t>
         </is>
       </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>external_id</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -781,7 +816,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -800,6 +835,11 @@
           <t>id</t>
         </is>
       </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>external_id</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -812,7 +852,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -851,6 +891,11 @@
           <t>id</t>
         </is>
       </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>external_id</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -863,7 +908,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -910,6 +955,11 @@
       <c r="H1" t="inlineStr">
         <is>
           <t>id</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>external_id</t>
         </is>
       </c>
     </row>
@@ -929,7 +979,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -971,6 +1021,11 @@
       <c r="G1" t="inlineStr">
         <is>
           <t>id</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>external_id</t>
         </is>
       </c>
     </row>
@@ -990,7 +1045,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1062,6 +1117,11 @@
       <c r="M1" t="inlineStr">
         <is>
           <t>id</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>external_id</t>
         </is>
       </c>
     </row>
@@ -1093,7 +1153,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1170,6 +1230,11 @@
       <c r="N1" t="inlineStr">
         <is>
           <t>id</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>external_id</t>
         </is>
       </c>
     </row>
@@ -1189,7 +1254,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1243,6 +1308,11 @@
           <t>id</t>
         </is>
       </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>external_id</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1255,7 +1325,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1292,6 +1362,11 @@
       <c r="F1" t="inlineStr">
         <is>
           <t>id</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>external_id</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🍱 Add Family and Sample Types
Adds family and sample classes (and supporting classes) in line with current best practices.
</commit_message>
<xml_diff>
--- a/project/excel/acr_harmonized_data_model.xlsx
+++ b/project/excel/acr_harmonized_data_model.xlsx
@@ -11,11 +11,16 @@
     <sheet name="AccessControlledRecord" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Study" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Sample" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Subject" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Demographics" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="SubjectAssertion" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="SourceData" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="AccessPolicy" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="BiospecimenCollection" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Aliquot" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Subject" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Demographics" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="SubjectAssertion" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="SourceData" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="AccessPolicy" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="Family" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="FamilyRelationship" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="FamilyMember" sheetId="14" state="visible" r:id="rId14"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -446,6 +451,312 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>code</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>display</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>value_code</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>value_display</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>value_number</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>value_units</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>value_units_display</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>has_access_policy</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>external_id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>data_access_type</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>access_policy_code</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>disease_limitation</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>website</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>external_id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"open,registered,controlled,gsr_restricted,gsr_allowed"</formula1>
+    </dataValidation>
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"gru,hmb,ds,irb,pub,col,npu,mds,gso,gsr"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>family_type</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>family_description</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>consanguinity</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>family_study_focus</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>family_members</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>family_relationships</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>has_access_policy</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>external_id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"control_only,duo,proband_only,trio,trio_plus,other"</formula1>
+    </dataValidation>
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"not_suspected,suspected,known_present,unknown"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>family_member</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>other_family_member</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>relationship_code</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>has_access_policy</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>external_id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>family_member</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>family_role</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>has_access_policy</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>external_id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -544,7 +855,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -555,12 +866,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>parent_sample_id</t>
+          <t>biospecimen_collection</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>biospecimen_collection_id_fk</t>
+          <t>parent_sample</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -585,15 +896,30 @@
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>quantity</t>
+          <t>quantity_number</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
+          <t>quantity_units</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>aliquots</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>has_access_policy</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>external_id</t>
         </is>
@@ -626,6 +952,147 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>age_at_collection</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>method</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>site</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>spatial_qualifier</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>laterality</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>has_access_policy</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>external_id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="4">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>""</formula1>
+    </dataValidation>
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>""</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>""</formula1>
+    </dataValidation>
+    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>""</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>availablity_status</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>quantity_number</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>quantity_units</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>concentration_number</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>concentration_unit</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>has_access_policy</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>external_id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"available,unavailable"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>subject_type</t>
         </is>
       </c>
@@ -675,7 +1142,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -783,7 +1250,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -882,139 +1349,4 @@
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>code</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>display</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>value_code</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>value_display</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>value_number</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>value_units</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>value_units_display</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>has_access_policy</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>external_id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>data_access_type</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>access_policy_code</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>disease_limitation</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>website</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>external_id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="2">
-    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"open,registered,controlled,gsr_restricted,gsr_allowed"</formula1>
-    </dataValidation>
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"gru,hmb,ds,irb,pub,col,npu,mds,gso,gsr"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
🍱  Add basic File implementation
* Adds basic file information into the model.
* Open-ended implementation of File Metadata for additional details.
* Fix SNOMED_CT references.
</commit_message>
<xml_diff>
--- a/project/excel/acr_harmonized_data_model.xlsx
+++ b/project/excel/acr_harmonized_data_model.xlsx
@@ -21,6 +21,8 @@
     <sheet name="Family" sheetId="12" state="visible" r:id="rId12"/>
     <sheet name="FamilyRelationship" sheetId="13" state="visible" r:id="rId13"/>
     <sheet name="FamilyMember" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="File" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="FileMetadata" sheetId="16" state="visible" r:id="rId16"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -757,6 +759,141 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>subject</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>filename</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>format</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>data_type</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>size</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>drs_uri</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>file_metadata</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>has_access_policy</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>external_id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>""</formula1>
+    </dataValidation>
+    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>""</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>code</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>display</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>value_code</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>value_display</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>external_id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Slight update to poetry integration
</commit_message>
<xml_diff>
--- a/project/excel/acr_harmonized_data_model.xlsx
+++ b/project/excel/acr_harmonized_data_model.xlsx
@@ -7,22 +7,21 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Thing" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="AccessControlledRecord" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Study" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Sample" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="BiospecimenCollection" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Aliquot" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Subject" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Demographics" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="SubjectAssertion" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="SourceData" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="AccessPolicy" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="Family" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="FamilyRelationship" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="FamilyMember" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="File" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="FileMetadata" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="AccessControlledRecord" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Study" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sample" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="BiospecimenCollection" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Aliquot" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Subject" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Demographics" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="SubjectAssertion" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="SourceData" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="AccessPolicy" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Family" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="FamilyRelationship" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="FamilyMember" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="File" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="FileMetadata" sheetId="15" state="visible" r:id="rId15"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -428,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,10 +438,15 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>has_access_policy</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>id</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>external_id</t>
         </is>
@@ -454,77 +458,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>code</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>display</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>value_code</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>value_display</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>value_number</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>value_units</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>value_units_display</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>has_access_policy</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>external_id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -588,7 +521,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -662,7 +595,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -713,7 +646,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -759,7 +692,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -843,7 +776,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -900,42 +833,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>has_access_policy</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>external_id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -986,7 +883,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1066,6 +963,81 @@
   <dataValidations count="1">
     <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"available,unavailable"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>age_at_collection</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>method</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>site</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>spatial_qualifier</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>laterality</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>has_access_policy</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>external_id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="4">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>""</formula1>
+    </dataValidation>
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>""</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>""</formula1>
+    </dataValidation>
+    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>""</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1089,27 +1061,27 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>age_at_collection</t>
+          <t>availablity_status</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>method</t>
+          <t>quantity_number</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>site</t>
+          <t>quantity_units</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>spatial_qualifier</t>
+          <t>concentration_number</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>laterality</t>
+          <t>concentration_unit</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
@@ -1129,18 +1101,9 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>""</formula1>
-    </dataValidation>
-    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>""</formula1>
-    </dataValidation>
-    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>""</formula1>
-    </dataValidation>
-    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>""</formula1>
+  <dataValidations count="1">
+    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"available,unavailable"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1164,72 +1127,6 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>availablity_status</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>quantity_number</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>quantity_units</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>concentration_number</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>concentration_unit</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>has_access_policy</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>external_id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"available,unavailable"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
           <t>subject_type</t>
         </is>
       </c>
@@ -1279,7 +1176,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1387,7 +1284,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1486,4 +1383,75 @@
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>code</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>display</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>value_code</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>value_display</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>value_number</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>value_units</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>value_units_display</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>has_access_policy</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>external_id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
✨ Add Source Data references
</commit_message>
<xml_diff>
--- a/project/excel/acr_harmonized_data_model.xlsx
+++ b/project/excel/acr_harmonized_data_model.xlsx
@@ -11,17 +11,18 @@
     <sheet name="Demographics" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Study" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="SubjectAssertion" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="SourceData" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="AccessPolicy" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Family" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="FamilyRelationship" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="FamilyMember" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="Sample" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="BiospecimenCollection" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="Aliquot" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="AccessControlledRecord" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="File" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="FileMetadata" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="DataSource" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="SourceData" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="AccessPolicy" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Family" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="FamilyRelationship" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="FamilyMember" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Sample" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="BiospecimenCollection" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="Aliquot" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="AccessControlledRecord" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="File" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="FileMetadata" sheetId="16" state="visible" r:id="rId16"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -493,6 +494,52 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>family_member</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>family_role</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>has_access_policy</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>external_id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -573,7 +620,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -648,7 +695,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -714,7 +761,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -750,7 +797,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -834,7 +881,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1156,72 +1203,103 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>code</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>display</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>value_code</t>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>snapshot_id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>google_data_project</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>snapshot_dataset</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>value_display</t>
+          <t>table</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>value_number</t>
+          <t>parameterized_query</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>value_units</t>
+          <t>id</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>value_units_display</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
+          <t>external_id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>data_source</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>query_parameter</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
         <is>
           <t>has_access_policy</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>external_id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>external_id</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1285,7 +1363,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1359,7 +1437,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1408,50 +1486,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>family_member</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>family_role</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>has_access_policy</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>external_id</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated to remove the External Study ID
</commit_message>
<xml_diff>
--- a/project/excel/acr_harmonized_data_model.xlsx
+++ b/project/excel/acr_harmonized_data_model.xlsx
@@ -1046,46 +1046,41 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>external_study_id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
         <is>
           <t>parent_study_id</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>funding_source</t>
         </is>
       </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>principal_investigator</t>
+        </is>
+      </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>principal_investigator</t>
+          <t>study_title</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>study_title</t>
+          <t>id</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
         <is>
           <t>external_id</t>
         </is>

</xml_diff>

<commit_message>
🔨 Add Related Diseases enumeration.
</commit_message>
<xml_diff>
--- a/project/excel/acr_harmonized_data_model.xlsx
+++ b/project/excel/acr_harmonized_data_model.xlsx
@@ -1185,7 +1185,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="A2:A1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"phenotypic_feature,disease,comorbidity,histology,clinical_finding,ehr_billing_code"</formula1>
+      <formula1>"phenotypic_feature,disease,comorbidity,histology,clinical_finding,ehr_billing_code,measurement"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1351,7 +1351,7 @@
       <formula1>"open,registered,controlled,gsr_restricted,gsr_allowed"</formula1>
     </dataValidation>
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"gru,hmb,ds,irb,pub,col,npu,mds,gso,gsr"</formula1>
+      <formula1>"gru,hmb,ds,irb,pub,col,npu,mds,gso,gsr,rd"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>